<commit_message>
Deploy 28d4dc4 from branch master
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Jahr</t>
   </si>
@@ -45,9 +45,6 @@
     <t>213 - 253</t>
   </si>
   <si>
-    <t>224 - 226</t>
-  </si>
-  <si>
     <t>223 - 265</t>
   </si>
   <si>
@@ -61,6 +58,15 @@
   </si>
   <si>
     <t>Deutsche Beobachtungsstelle für Drogen und Drogensucht (DBDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkung: </t>
+  </si>
+  <si>
+    <t>Geschätzte Werte</t>
+  </si>
+  <si>
+    <t>224 - 266</t>
   </si>
 </sst>
 </file>
@@ -172,11 +178,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185112064"/>
-        <c:axId val="40676736"/>
+        <c:axId val="182031872"/>
+        <c:axId val="41463168"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="185112064"/>
+        <c:axId val="182031872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40676736"/>
+        <c:crossAx val="41463168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -423,7 +429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40676736"/>
+        <c:axId val="41463168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185112064"/>
+        <c:crossAx val="182031872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -883,7 +889,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,23 +920,23 @@
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1008,7 +1014,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1021,7 +1027,7 @@
         <v>2016</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1031,7 +1037,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1228,8 +1234,12 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1241,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="1"/>
@@ -1324,7 +1334,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deploy 0af85f9 from branch master
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="13290"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Gerundet" sheetId="1" r:id="rId1"/>
+    <sheet name="Exakt" sheetId="4" r:id="rId2"/>
+    <sheet name="Daten" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Jahr</t>
   </si>
@@ -33,22 +33,7 @@
     <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangaben gestattet.</t>
   </si>
   <si>
-    <t>214 - 254</t>
-  </si>
-  <si>
-    <t>229 - 272</t>
-  </si>
-  <si>
     <t>217 - 258</t>
-  </si>
-  <si>
-    <t>213 - 253</t>
-  </si>
-  <si>
-    <t>223 - 265</t>
-  </si>
-  <si>
-    <t>Behandlungsnachfrage in Suchtzentren (Stoffgruppen Opioide, Kokain und Stimulanzien) in der Altersklasse 18 bis unter 65 Jahre</t>
   </si>
   <si>
     <t>Werte in 1 000</t>
@@ -66,7 +51,46 @@
     <t>Geschätzte Werte</t>
   </si>
   <si>
-    <t>224 - 266</t>
+    <t>231 - 274</t>
+  </si>
+  <si>
+    <t>218 - 259</t>
+  </si>
+  <si>
+    <t>215 - 255</t>
+  </si>
+  <si>
+    <t>225 - 268</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>215 078 - 255 405</t>
+  </si>
+  <si>
+    <t>231 052 - 274 374</t>
+  </si>
+  <si>
+    <t>218 360 - 259 303</t>
+  </si>
+  <si>
+    <t>215 436 - 255 830</t>
+  </si>
+  <si>
+    <t>230 672 - 273 923</t>
+  </si>
+  <si>
+    <t>225 471 - 267 747</t>
+  </si>
+  <si>
+    <t>225 324 - 267 572</t>
+  </si>
+  <si>
+    <t>217 220 - 257 949</t>
+  </si>
+  <si>
+    <t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</t>
   </si>
 </sst>
 </file>
@@ -158,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -178,9 +202,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -224,13 +245,39 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1400"/>
-              <a:t>Behandlungsnachfrage in Suchtzentren (Stoffgruppen Opioide, Kokain und Stimulanzien) in der Altersklasse 18 bis unter 65 Jahre</a:t>
+              <a:rPr lang="de-DE" sz="1400" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
             </a:r>
+            <a:endParaRPr lang="de-DE" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -251,10 +298,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:f>Daten!$A$1:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -275,36 +322,42 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$1:$B$7</c:f>
+              <c:f>Daten!$B$1:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>214</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>229</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -320,10 +373,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:f>Daten!$A$1:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -344,16 +397,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$C$1:$C$7</c:f>
+              <c:f>Daten!$C$1:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -364,16 +420,19 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,11 +446,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182031872"/>
-        <c:axId val="41463168"/>
+        <c:axId val="177116672"/>
+        <c:axId val="41594240"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="182031872"/>
+        <c:axId val="177116672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41463168"/>
+        <c:crossAx val="41594240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -429,7 +488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41463168"/>
+        <c:axId val="41594240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,7 +518,291 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182031872"/>
+        <c:crossAx val="177116672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400"/>
+              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Daten!$A$1:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Daten!$H$1:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>215078</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>231052</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>218360</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230672</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225471</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>217220</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4C9F38"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Daten!$A$1:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Daten!$I$1:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>40327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43322</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40943</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42276</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="158196224"/>
+        <c:axId val="41597120"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="158196224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Jahr</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41597120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41597120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0;\-#\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="158196224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -587,6 +930,131 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="911088" y="7810499"/>
+          <a:ext cx="142857" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1245</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1201588</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1245"/>
+          <a:ext cx="1971871" cy="713130"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>140805</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>283662</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="912330" y="7813812"/>
           <a:ext cx="142857" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -888,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +1377,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -918,25 +1386,25 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -949,7 +1417,7 @@
         <v>2010</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -962,7 +1430,7 @@
         <v>2011</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -975,7 +1443,7 @@
         <v>2012</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -988,7 +1456,7 @@
         <v>2013</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1001,7 +1469,7 @@
         <v>2014</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1014,7 +1482,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1027,7 +1495,7 @@
         <v>2016</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1036,8 +1504,12 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1235,10 +1707,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1251,7 +1723,457 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="1"/>
@@ -1329,137 +2251,233 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>2010</v>
       </c>
       <c r="B1">
-        <v>214</v>
+        <f t="shared" ref="B1:B8" si="0">ROUND(H1/1000,0)</f>
+        <v>215</v>
       </c>
       <c r="C1">
         <f>D1-B1</f>
         <v>40</v>
       </c>
       <c r="D1">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <f>ROUND(J1/1000,0)</f>
+        <v>255</v>
+      </c>
+      <c r="H1">
+        <v>215078</v>
+      </c>
+      <c r="I1">
+        <f>J1-H1</f>
+        <v>40327</v>
+      </c>
+      <c r="J1">
+        <v>255405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>229</v>
+        <f t="shared" si="0"/>
+        <v>231</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C7" si="0">D2-B2</f>
+        <f t="shared" ref="C2:C8" si="1">D2-B2</f>
         <v>43</v>
       </c>
       <c r="D2">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D2:D8" si="2">ROUND(J2/1000,0)</f>
+        <v>274</v>
+      </c>
+      <c r="H2">
+        <v>231052</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I8" si="3">J2-H2</f>
+        <v>43322</v>
+      </c>
+      <c r="J2">
+        <v>274374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>217</v>
+        <f t="shared" si="0"/>
+        <v>218</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D3">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="H3">
+        <v>218360</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="3"/>
+        <v>40943</v>
+      </c>
+      <c r="J3">
+        <v>259303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>213</v>
+        <f t="shared" si="0"/>
+        <v>215</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="D4">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="H4">
+        <v>215436</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>40394</v>
+      </c>
+      <c r="J4">
+        <v>255830</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>229</v>
+        <f t="shared" si="0"/>
+        <v>231</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="D5">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <f>ROUND(J5/1000,0)</f>
+        <v>274</v>
+      </c>
+      <c r="H5">
+        <v>230672</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>43251</v>
+      </c>
+      <c r="J5">
+        <v>273923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>224</v>
+        <f t="shared" si="0"/>
+        <v>225</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>268</v>
+      </c>
+      <c r="H6">
+        <v>225471</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>42276</v>
+      </c>
+      <c r="J6">
+        <v>267747</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>223</v>
+        <f t="shared" si="0"/>
+        <v>225</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>268</v>
+      </c>
+      <c r="H7">
+        <v>225324</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>42248</v>
+      </c>
+      <c r="J7">
+        <v>267572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B8">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="D7">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+        <v>217</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>258</v>
+      </c>
+      <c r="H8">
+        <v>217220</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>40729</v>
+      </c>
+      <c r="J8">
+        <v>257949</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to master from  @ 09938b2f6a247797ca652037f3df23a860d9218b 🚀
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dauerausleihe04\Documents\SDG\SdgTestEnvironment\sdg-indicators\public\AddInfos\de\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA720380-770B-40B6-B6C6-BDA01EEBAA38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="28512" windowHeight="13296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gerundet" sheetId="1" r:id="rId1"/>
     <sheet name="Exakt" sheetId="4" r:id="rId2"/>
     <sheet name="Daten" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Jahr</t>
   </si>
@@ -92,11 +98,14 @@
   <si>
     <t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</t>
   </si>
+  <si>
+    <t>©       Statistisches Bundesamt (Destatis) 2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,12 +230,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -281,7 +293,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -362,6 +373,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E537-441D-9001-EFA4B70F694C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -437,6 +453,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E537-441D-9001-EFA4B70F694C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -473,7 +494,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -511,7 +531,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -536,7 +555,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -565,7 +584,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -646,6 +664,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2DF-43C6-B66A-440CBBE3CD79}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -721,6 +744,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2DF-43C6-B66A-440CBBE3CD79}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -741,25 +769,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Jahr</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -795,7 +804,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#\ ##0;\-#\ ##0" sourceLinked="0"/>
@@ -836,7 +844,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -866,7 +880,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Grafik 4"/>
+        <xdr:cNvPr id="5" name="Grafik 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -910,7 +930,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Grafik 6"/>
+        <xdr:cNvPr id="7" name="Grafik 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -959,7 +985,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -991,7 +1023,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1035,7 +1073,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1068,9 +1112,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1108,9 +1152,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1143,9 +1187,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1178,9 +1239,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1353,22 +1431,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1377,7 +1455,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1386,7 +1464,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1477,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1490,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
@@ -1425,7 +1503,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2011</v>
       </c>
@@ -1438,7 +1516,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2012</v>
       </c>
@@ -1451,7 +1529,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -1464,7 +1542,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2014</v>
       </c>
@@ -1477,7 +1555,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2015</v>
       </c>
@@ -1490,7 +1568,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2016</v>
       </c>
@@ -1503,7 +1581,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2017</v>
       </c>
@@ -1516,7 +1594,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1525,7 +1603,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1534,7 +1612,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1543,7 +1621,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1552,7 +1630,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1561,7 +1639,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1570,7 +1648,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1579,7 +1657,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1588,7 +1666,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1597,7 +1675,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1606,7 +1684,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1615,7 +1693,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1624,7 +1702,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1633,7 +1711,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1642,7 +1720,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1651,7 +1729,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1660,7 +1738,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1669,7 +1747,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1678,7 +1756,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1687,7 +1765,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1696,7 +1774,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1705,7 +1783,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1796,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1809,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>2</v>
       </c>
@@ -1744,7 +1822,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7" t="s">
         <v>4</v>
@@ -1755,7 +1833,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1764,7 +1842,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1773,7 +1851,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1782,7 +1860,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1802,23 +1880,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1827,7 +1905,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1836,7 +1914,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1849,7 +1927,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1940,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
@@ -1875,7 +1953,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2011</v>
       </c>
@@ -1888,7 +1966,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2012</v>
       </c>
@@ -1901,7 +1979,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -1914,7 +1992,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2014</v>
       </c>
@@ -1927,7 +2005,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2015</v>
       </c>
@@ -1940,7 +2018,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2016</v>
       </c>
@@ -1953,7 +2031,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2017</v>
       </c>
@@ -1966,7 +2044,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1975,7 +2053,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1984,7 +2062,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1993,7 +2071,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2002,7 +2080,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2011,7 +2089,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2020,7 +2098,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2029,7 +2107,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2038,7 +2116,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2047,7 +2125,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2056,7 +2134,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2065,7 +2143,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2074,7 +2152,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2083,7 +2161,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2092,7 +2170,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2101,7 +2179,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2110,7 +2188,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2119,7 +2197,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2128,7 +2206,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2137,7 +2215,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2146,7 +2224,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2155,7 +2233,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>9</v>
       </c>
@@ -2168,7 +2246,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>1</v>
       </c>
@@ -2181,12 +2259,12 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
@@ -2194,7 +2272,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7" t="s">
         <v>4</v>
@@ -2205,7 +2283,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2214,7 +2292,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2223,7 +2301,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2232,7 +2310,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2252,16 +2330,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>2010</v>
       </c>
@@ -2288,7 +2366,7 @@
         <v>255405</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>2011</v>
       </c>
@@ -2315,7 +2393,7 @@
         <v>274374</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2012</v>
       </c>
@@ -2342,7 +2420,7 @@
         <v>259303</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2013</v>
       </c>
@@ -2369,7 +2447,7 @@
         <v>255830</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2014</v>
       </c>
@@ -2396,7 +2474,7 @@
         <v>273923</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
@@ -2423,7 +2501,7 @@
         <v>267747</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2016</v>
       </c>
@@ -2450,7 +2528,7 @@
         <v>267572</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2017</v>
       </c>

</xml_diff>

<commit_message>
Deploying to master from  @ 49eec29d74750ed9b5b8f29b2f6d9df7c35aff3f 🚀
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dauerausleihe04\Documents\SDG\SdgTestEnvironment\sdg-indicators\public\AddInfos\de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA720380-770B-40B6-B6C6-BDA01EEBAA38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86E978-58B2-427C-B7D4-8F24606ABCFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="96" windowWidth="28512" windowHeight="13296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Jahr</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>©       Statistisches Bundesamt (Destatis) 2021</t>
+  </si>
+  <si>
+    <t>218 - 258</t>
+  </si>
+  <si>
+    <t>204 906 - 243 326</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Daten!$A$1:$A$8</c:f>
+              <c:f>Daten!$A$1:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -627,16 +633,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$H$1:$H$8</c:f>
+              <c:f>Daten!$H$1:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>215078</c:v>
                 </c:pt>
@@ -660,6 +669,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>217220</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>204906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,10 +692,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Daten!$A$1:$A$8</c:f>
+              <c:f>Daten!$A$1:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -707,16 +719,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$I$1:$I$8</c:f>
+              <c:f>Daten!$I$1:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40327</c:v>
                 </c:pt>
@@ -740,6 +755,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>40729</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38420</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,13 +851,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -874,7 +892,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>257371</xdr:colOff>
+      <xdr:colOff>249751</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -919,14 +937,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>140805</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>283662</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>184269</xdr:rowOff>
+      <xdr:colOff>287472</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -974,13 +992,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1062,14 +1080,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>140805</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>283662</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>184269</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1432,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,8 +1613,12 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1784,12 +1806,8 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1798,12 +1816,12 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1811,10 +1829,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
@@ -1823,9 +1841,11 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7" t="s">
-        <v>4</v>
+      <c r="A37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
@@ -1834,9 +1854,11 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1868,6 +1890,15 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1881,19 +1912,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1914,7 +1944,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2045,8 +2075,12 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2234,12 +2268,8 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2248,12 +2278,12 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2261,10 +2291,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
@@ -2273,9 +2303,11 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7" t="s">
-        <v>4</v>
+      <c r="A37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
@@ -2284,9 +2316,11 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2319,22 +2353,31 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2375,7 +2418,7 @@
         <v>231</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C8" si="1">D2-B2</f>
+        <f t="shared" ref="C2:C9" si="1">D2-B2</f>
         <v>43</v>
       </c>
       <c r="D2">
@@ -2386,7 +2429,7 @@
         <v>231052</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I8" si="3">J2-H2</f>
+        <f t="shared" ref="I2:I9" si="3">J2-H2</f>
         <v>43322</v>
       </c>
       <c r="J2">
@@ -2537,7 +2580,7 @@
         <v>217</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f>D8-B8</f>
         <v>41</v>
       </c>
       <c r="D8">
@@ -2553,6 +2596,31 @@
       </c>
       <c r="J8">
         <v>257949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B9">
+        <v>205</v>
+      </c>
+      <c r="C9">
+        <f>D9-B9</f>
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>243</v>
+      </c>
+      <c r="H9">
+        <v>204906</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>38420</v>
+      </c>
+      <c r="J9">
+        <v>243326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to master from  @ 05a6cca6221a7aaccd2289268cca00b692f0caef 🚀
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dauerausleihe04\Documents\SDG\SdgTestEnvironment\sdg-indicators\public\AddInfos\de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86E978-58B2-427C-B7D4-8F24606ABCFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766EAB0-18ED-4B14-9840-6B5EE2A9FE9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="28512" windowHeight="13296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gerundet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Jahr</t>
   </si>
@@ -99,13 +99,28 @@
     <t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</t>
   </si>
   <si>
-    <t>©       Statistisches Bundesamt (Destatis) 2021</t>
-  </si>
-  <si>
     <t>218 - 258</t>
   </si>
   <si>
     <t>204 906 - 243 326</t>
+  </si>
+  <si>
+    <t>© Statistisches Bundesamt (Destatis) 2021</t>
+  </si>
+  <si>
+    <t>Deutsche Beobachtungsstelle für Drogen und Drogensucht</t>
+  </si>
+  <si>
+    <t>Geographische Abdeckung:</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>Einheit:</t>
+  </si>
+  <si>
+    <t>Geschätzte Werte.</t>
   </si>
 </sst>
 </file>
@@ -197,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +233,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -996,7 +1017,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1035,9 +1056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1201588</xdr:colOff>
+      <xdr:colOff>460543</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1068,56 +1089,6 @@
         <a:xfrm>
           <a:off x="0" y="1245"/>
           <a:ext cx="1971871" cy="713130"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>140805</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>41412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>283662</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>1389</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="912330" y="7813812"/>
-          <a:ext cx="142857" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1456,15 +1427,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1473,7 +1444,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1482,7 +1453,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1466,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1479,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
@@ -1521,7 +1492,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2011</v>
       </c>
@@ -1534,7 +1505,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2012</v>
       </c>
@@ -1547,7 +1518,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -1560,7 +1531,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2014</v>
       </c>
@@ -1573,7 +1544,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2015</v>
       </c>
@@ -1586,7 +1557,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2016</v>
       </c>
@@ -1599,7 +1570,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2017</v>
       </c>
@@ -1612,12 +1583,12 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2018</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1625,7 +1596,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1634,7 +1605,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1643,7 +1614,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1652,7 +1623,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1661,7 +1632,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1670,7 +1641,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1679,7 +1650,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1688,7 +1659,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1697,7 +1668,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1706,7 +1677,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1715,7 +1686,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1724,7 +1695,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1733,7 +1704,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1742,7 +1713,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1751,7 +1722,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1760,7 +1731,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1769,7 +1740,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1778,7 +1749,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1787,7 +1758,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1796,7 +1767,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1805,7 +1776,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1814,7 +1785,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>9</v>
       </c>
@@ -1827,7 +1798,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
@@ -1840,7 +1811,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>2</v>
       </c>
@@ -1853,7 +1824,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7" t="s">
         <v>4</v>
@@ -1864,7 +1835,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1873,7 +1844,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1882,7 +1853,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1891,7 +1862,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1912,21 +1883,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="6" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1935,7 +1906,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1944,7 +1915,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1955,9 +1926,9 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1970,7 +1941,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
@@ -1983,7 +1954,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2011</v>
       </c>
@@ -1996,7 +1967,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2012</v>
       </c>
@@ -2009,7 +1980,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -2022,7 +1993,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2014</v>
       </c>
@@ -2035,7 +2006,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2015</v>
       </c>
@@ -2048,7 +2019,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2016</v>
       </c>
@@ -2061,7 +2032,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2017</v>
       </c>
@@ -2074,12 +2045,12 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2018</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2087,7 +2058,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2096,7 +2067,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2105,7 +2076,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2114,7 +2085,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2123,7 +2094,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2132,7 +2103,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2141,7 +2112,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2150,7 +2121,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2159,7 +2130,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2168,7 +2139,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2177,7 +2148,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2186,7 +2157,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2195,7 +2166,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2204,7 +2175,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2213,7 +2184,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2222,7 +2193,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2231,7 +2202,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2240,7 +2211,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2249,7 +2220,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2258,7 +2229,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2267,7 +2238,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2276,25 +2247,25 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="C35" s="7"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
@@ -2302,12 +2273,12 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
@@ -2315,36 +2286,44 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="B38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="7"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+    <row r="40" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2353,7 +2332,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2362,9 +2341,28 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:G3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2380,9 +2378,9 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>2010</v>
       </c>
@@ -2409,7 +2407,7 @@
         <v>255405</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2011</v>
       </c>
@@ -2418,7 +2416,7 @@
         <v>231</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C9" si="1">D2-B2</f>
+        <f t="shared" ref="C2:C7" si="1">D2-B2</f>
         <v>43</v>
       </c>
       <c r="D2">
@@ -2436,7 +2434,7 @@
         <v>274374</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2012</v>
       </c>
@@ -2463,7 +2461,7 @@
         <v>259303</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2013</v>
       </c>
@@ -2490,7 +2488,7 @@
         <v>255830</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2014</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>273923</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
@@ -2544,7 +2542,7 @@
         <v>267747</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2016</v>
       </c>
@@ -2571,7 +2569,7 @@
         <v>267572</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2017</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>257949</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2018</v>
       </c>

</xml_diff>